<commit_message>
Add Quadratic Report template as pptx
</commit_message>
<xml_diff>
--- a/inst/data-demo/conjoint_data.xlsx
+++ b/inst/data-demo/conjoint_data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t>start</t>
   </si>
@@ -463,9 +463,6 @@
   </si>
   <si>
     <t>17.00695000216365</t>
-  </si>
-  <si>
-    <t>usr18</t>
   </si>
   <si>
     <t>e5839971-6a21-4f4e-9831-2f4157c8e93b</t>
@@ -521,10 +518,13 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1041,6 +1041,7 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" min="1" max="3" width="9.8515625"/>
+    <col customWidth="1" min="6" max="6" width="29.8515625"/>
     <col customWidth="1" min="7" max="7" width="32.7109375"/>
     <col bestFit="1" min="52" max="52" width="9.8515625"/>
   </cols>
@@ -3827,8 +3828,8 @@
       <c r="F19" t="s">
         <v>149</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>150</v>
+      <c r="G19" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="M19">
         <v>1</v>
@@ -3945,7 +3946,7 @@
         <v>27790492</v>
       </c>
       <c r="AY19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AZ19" s="1">
         <v>45008.666238425933</v>
@@ -3971,16 +3972,16 @@
         <v>45007</v>
       </c>
       <c r="D20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" t="s">
         <v>152</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>153</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -4097,7 +4098,7 @@
         <v>27790441</v>
       </c>
       <c r="AY20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AZ20" s="1">
         <v>45008.663611111107</v>

</xml_diff>